<commit_message>
new files for helper excel sheet
</commit_message>
<xml_diff>
--- a/tests/testsample.xlsx
+++ b/tests/testsample.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\languages\VBS\uft\advanceduft\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367C94B8-750D-4D98-A144-A66DE07F9ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-20865" yWindow="2205" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Steps" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,7 +336,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
updating to automate local/remote load and run
</commit_message>
<xml_diff>
--- a/tests/testsample.xlsx
+++ b/tests/testsample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\languages\VBS\uft\advanceduft\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367C94B8-750D-4D98-A144-A66DE07F9ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F4F135-8D3E-447B-9704-3189613A94B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20865" yWindow="2205" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19860" yWindow="1680" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,63 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+  <si>
+    <t>STEP_ID</t>
+  </si>
+  <si>
+    <t>ACTION_NAME</t>
+  </si>
+  <si>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t>DATASHEET</t>
+  </si>
+  <si>
+    <t>ITERATIONS</t>
+  </si>
+  <si>
+    <t>ON_FAILURE</t>
+  </si>
+  <si>
+    <t>Open Browser</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>ExitTest</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>STORE_RESULT_AS</t>
+  </si>
+  <si>
+    <t>Close Browser</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -55,8 +106,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,12 +389,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
making this less problematic to use
</commit_message>
<xml_diff>
--- a/tests/testsample.xlsx
+++ b/tests/testsample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\languages\VBS\uft\advanceduft\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F4F135-8D3E-447B-9704-3189613A94B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFCC973-5239-4134-889C-D081A5CC28D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19860" yWindow="1680" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24060" yWindow="825" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>VALUE</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>ExitTest</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Close Browser</t>
+  </si>
+  <si>
+    <t>FIREFOX</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -441,13 +441,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -455,16 +455,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>